<commit_message>
new models treeD, C5 and randF
</commit_message>
<xml_diff>
--- a/AppsRating/submission/resultado.xlsx
+++ b/AppsRating/submission/resultado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>ImputaciónMediana</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,7 +386,7 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +399,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -410,8 +416,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -424,8 +433,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -437,6 +449,9 @@
       </c>
       <c r="D4" t="s">
         <v>7</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>